<commit_message>
Great work on email sending
</commit_message>
<xml_diff>
--- a/Matched groups.xlsx
+++ b/Matched groups.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="424">
   <si>
     <t>Community Member Name</t>
   </si>
@@ -214,6 +214,30 @@
     <t>Sunday October 1st - 9:00-12:00</t>
   </si>
   <si>
+    <t>Person 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email4@queensu.ca </t>
+  </si>
+  <si>
+    <t>100 University Avenue</t>
+  </si>
+  <si>
+    <t>2017-09-27 13:59:02</t>
+  </si>
+  <si>
+    <t>Volunteer 107</t>
+  </si>
+  <si>
+    <t>Volunteer 181</t>
+  </si>
+  <si>
+    <t>Volunteer 242</t>
+  </si>
+  <si>
+    <t>Volunteer 295</t>
+  </si>
+  <si>
     <t>Person 5</t>
   </si>
   <si>
@@ -358,6 +382,33 @@
     <t>peanut allergy</t>
   </si>
   <si>
+    <t>Person 9</t>
+  </si>
+  <si>
+    <t>613-533-0007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email8@queensu.ca </t>
+  </si>
+  <si>
+    <t>1893 Spindlewood Street</t>
+  </si>
+  <si>
+    <t>2017-09-18 22:14:58</t>
+  </si>
+  <si>
+    <t>Volunteer 11</t>
+  </si>
+  <si>
+    <t>Volunteer 119</t>
+  </si>
+  <si>
+    <t>Volunteer 189</t>
+  </si>
+  <si>
+    <t>Volunteer 250</t>
+  </si>
+  <si>
     <t>Person 10</t>
   </si>
   <si>
@@ -427,6 +478,9 @@
     <t>Clean garage, paper shredding, sort books</t>
   </si>
   <si>
+    <t>75 Bader Lane</t>
+  </si>
+  <si>
     <t>2017-09-26 23:48:58</t>
   </si>
   <si>
@@ -457,19 +511,19 @@
     <t>43 Markland Street</t>
   </si>
   <si>
-    <t>2017-09-27 13:59:02</t>
-  </si>
-  <si>
-    <t>Volunteer 107</t>
-  </si>
-  <si>
-    <t>Volunteer 181</t>
-  </si>
-  <si>
-    <t>Volunteer 242</t>
-  </si>
-  <si>
-    <t>Volunteer 295</t>
+    <t>2017-09-25 19:33:59</t>
+  </si>
+  <si>
+    <t>Volunteer 76</t>
+  </si>
+  <si>
+    <t>Volunteer 158</t>
+  </si>
+  <si>
+    <t>Volunteer 223</t>
+  </si>
+  <si>
+    <t>Volunteer 279</t>
   </si>
   <si>
     <t>Person 14</t>
@@ -511,22 +565,79 @@
     <t xml:space="preserve">email10@queensu.ca </t>
   </si>
   <si>
-    <t>314 Emerald Street, Kingston ON</t>
-  </si>
-  <si>
-    <t>2017-09-25 19:33:59</t>
-  </si>
-  <si>
-    <t>Volunteer 76</t>
-  </si>
-  <si>
-    <t>Volunteer 158</t>
-  </si>
-  <si>
-    <t>Volunteer 223</t>
-  </si>
-  <si>
-    <t>Volunteer 279</t>
+    <t>314 Emerald Street</t>
+  </si>
+  <si>
+    <t>2017-09-19 13:53:42</t>
+  </si>
+  <si>
+    <t>Volunteer 19</t>
+  </si>
+  <si>
+    <t>Volunteer 122</t>
+  </si>
+  <si>
+    <t>Volunteer 191</t>
+  </si>
+  <si>
+    <t>Volunteer 252</t>
+  </si>
+  <si>
+    <t>Volunteer 301</t>
+  </si>
+  <si>
+    <t>Allergies to animals</t>
+  </si>
+  <si>
+    <t>Person 16</t>
+  </si>
+  <si>
+    <t>613-533-0014</t>
+  </si>
+  <si>
+    <t>furniture moved and floors vacuumed/cleaned. Likely some other shit</t>
+  </si>
+  <si>
+    <t>1247 Unity Road</t>
+  </si>
+  <si>
+    <t>2017-09-26 23:50:48</t>
+  </si>
+  <si>
+    <t>Volunteer 99</t>
+  </si>
+  <si>
+    <t>Volunteer 173</t>
+  </si>
+  <si>
+    <t>Volunteer 234</t>
+  </si>
+  <si>
+    <t>Volunteer 287</t>
+  </si>
+  <si>
+    <t>and thats it</t>
+  </si>
+  <si>
+    <t>Person 17</t>
+  </si>
+  <si>
+    <t>613-533-0015</t>
+  </si>
+  <si>
+    <t>2017-09-19 21:48:27</t>
+  </si>
+  <si>
+    <t>Volunteer 23</t>
+  </si>
+  <si>
+    <t>Volunteer 124</t>
+  </si>
+  <si>
+    <t>Volunteer 193</t>
+  </si>
+  <si>
+    <t>Volunteer 254</t>
   </si>
   <si>
     <t>Person 18</t>
@@ -541,19 +652,22 @@
     <t>72 Herchmer Cres</t>
   </si>
   <si>
-    <t>2017-09-19 21:48:27</t>
-  </si>
-  <si>
-    <t>Volunteer 23</t>
-  </si>
-  <si>
-    <t>Volunteer 124</t>
-  </si>
-  <si>
-    <t>Volunteer 193</t>
-  </si>
-  <si>
-    <t>Volunteer 254</t>
+    <t>2017-09-25 08:22:23</t>
+  </si>
+  <si>
+    <t>Volunteer 61</t>
+  </si>
+  <si>
+    <t>Volunteer 145</t>
+  </si>
+  <si>
+    <t>Volunteer 212</t>
+  </si>
+  <si>
+    <t>Volunteer 271</t>
+  </si>
+  <si>
+    <t>Volunteer 314</t>
   </si>
   <si>
     <t>Person 19</t>
@@ -568,22 +682,22 @@
     <t>4 Greensboro Ave</t>
   </si>
   <si>
-    <t>2017-09-25 08:22:23</t>
-  </si>
-  <si>
-    <t>Volunteer 61</t>
-  </si>
-  <si>
-    <t>Volunteer 145</t>
-  </si>
-  <si>
-    <t>Volunteer 212</t>
-  </si>
-  <si>
-    <t>Volunteer 271</t>
-  </si>
-  <si>
-    <t>Volunteer 314</t>
+    <t>2017-09-19 14:12:23</t>
+  </si>
+  <si>
+    <t>Volunteer 20</t>
+  </si>
+  <si>
+    <t>Volunteer 123</t>
+  </si>
+  <si>
+    <t>Volunteer 192</t>
+  </si>
+  <si>
+    <t>Volunteer 253</t>
+  </si>
+  <si>
+    <t>Volunteer 302</t>
   </si>
   <si>
     <t>Person 20</t>
@@ -601,88 +715,19 @@
     <t>Realistically only needs 2 people</t>
   </si>
   <si>
-    <t>2017-09-19 13:53:42</t>
-  </si>
-  <si>
-    <t>Volunteer 19</t>
-  </si>
-  <si>
-    <t>Volunteer 122</t>
-  </si>
-  <si>
-    <t>Volunteer 191</t>
-  </si>
-  <si>
-    <t>Volunteer 252</t>
-  </si>
-  <si>
-    <t>Volunteer 301</t>
-  </si>
-  <si>
-    <t>Allergies to animals</t>
-  </si>
-  <si>
-    <t>Person 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email4@queensu.ca </t>
-  </si>
-  <si>
-    <t>1508 Clover</t>
-  </si>
-  <si>
-    <t>Person 9</t>
-  </si>
-  <si>
-    <t>613-533-0007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email8@queensu.ca </t>
-  </si>
-  <si>
-    <t>1893 Spindlewood Street</t>
-  </si>
-  <si>
-    <t>Person 16</t>
-  </si>
-  <si>
-    <t>613-533-0014</t>
-  </si>
-  <si>
-    <t>saturday afternoon</t>
-  </si>
-  <si>
-    <t>furniture moved and floors vacuumed/cleaned. Likely some other shit</t>
-  </si>
-  <si>
-    <t>1247 Unity Road</t>
-  </si>
-  <si>
-    <t>Person 17</t>
-  </si>
-  <si>
-    <t>613-533-0015</t>
-  </si>
-  <si>
-    <t>DRIVE SO TOLD HER SATURDAY MORNING ONLY</t>
-  </si>
-  <si>
-    <t>2017-09-26 23:50:48</t>
-  </si>
-  <si>
-    <t>Volunteer 99</t>
-  </si>
-  <si>
-    <t>Volunteer 173</t>
-  </si>
-  <si>
-    <t>Volunteer 234</t>
-  </si>
-  <si>
-    <t>Volunteer 287</t>
-  </si>
-  <si>
-    <t>and thats it</t>
+    <t>2017-09-25 19:36:32</t>
+  </si>
+  <si>
+    <t>Volunteer 77</t>
+  </si>
+  <si>
+    <t>Volunteer 159</t>
+  </si>
+  <si>
+    <t>Volunteer 224</t>
+  </si>
+  <si>
+    <t>Volunteer 280</t>
   </si>
   <si>
     <t>2017-09-27 22:44:11</t>
@@ -706,21 +751,6 @@
     <t>We have two more members: Rachel Churko (17rkc1@queensu.ca) and Abby Dusome (16ald9@queensu.ca).</t>
   </si>
   <si>
-    <t>2017-09-18 22:14:58</t>
-  </si>
-  <si>
-    <t>Volunteer 11</t>
-  </si>
-  <si>
-    <t>Volunteer 119</t>
-  </si>
-  <si>
-    <t>Volunteer 189</t>
-  </si>
-  <si>
-    <t>Volunteer 250</t>
-  </si>
-  <si>
     <t>2017-09-18 22:10:37</t>
   </si>
   <si>
@@ -796,24 +826,6 @@
     <t>Volunteer 324</t>
   </si>
   <si>
-    <t>2017-09-19 14:12:23</t>
-  </si>
-  <si>
-    <t>Volunteer 20</t>
-  </si>
-  <si>
-    <t>Volunteer 123</t>
-  </si>
-  <si>
-    <t>Volunteer 192</t>
-  </si>
-  <si>
-    <t>Volunteer 253</t>
-  </si>
-  <si>
-    <t>Volunteer 302</t>
-  </si>
-  <si>
     <t>2017-09-19 21:53:32</t>
   </si>
   <si>
@@ -1100,21 +1112,6 @@
   </si>
   <si>
     <t>Volunteer 320</t>
-  </si>
-  <si>
-    <t>2017-09-25 19:36:32</t>
-  </si>
-  <si>
-    <t>Volunteer 77</t>
-  </si>
-  <si>
-    <t>Volunteer 159</t>
-  </si>
-  <si>
-    <t>Volunteer 224</t>
-  </si>
-  <si>
-    <t>Volunteer 280</t>
   </si>
   <si>
     <t>2017-09-22 08:40:30</t>
@@ -1620,7 +1617,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA96"/>
+  <dimension ref="A1:AA57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1887,53 +1884,47 @@
       <c r="A5" t="s">
         <v>66</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
       </c>
       <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" t="s">
         <v>69</v>
       </c>
-      <c r="H5" t="s">
+      <c r="M5" t="s">
         <v>70</v>
       </c>
-      <c r="I5" t="s">
+      <c r="N5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" t="s">
         <v>71</v>
       </c>
-      <c r="L5" t="s">
+      <c r="P5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" t="s">
         <v>72</v>
       </c>
-      <c r="M5" t="s">
+      <c r="R5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" t="s">
         <v>73</v>
       </c>
-      <c r="N5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O5" t="s">
-        <v>74</v>
-      </c>
-      <c r="P5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>75</v>
-      </c>
-      <c r="R5" t="s">
-        <v>35</v>
-      </c>
-      <c r="S5" t="s">
-        <v>76</v>
-      </c>
       <c r="T5" t="s">
         <v>35</v>
       </c>
       <c r="W5" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="X5" t="s">
         <v>40</v>
@@ -1944,303 +1935,303 @@
     </row>
     <row r="6" spans="1:27">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="H6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" t="s">
+        <v>79</v>
+      </c>
+      <c r="L6" t="s">
+        <v>80</v>
+      </c>
+      <c r="M6" t="s">
         <v>81</v>
       </c>
-      <c r="I6" t="s">
+      <c r="N6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" t="s">
         <v>82</v>
       </c>
-      <c r="L6" t="s">
+      <c r="P6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" t="s">
         <v>83</v>
       </c>
-      <c r="M6" t="s">
+      <c r="R6" t="s">
+        <v>35</v>
+      </c>
+      <c r="S6" t="s">
         <v>84</v>
       </c>
-      <c r="N6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="T6" t="s">
+        <v>35</v>
+      </c>
+      <c r="W6" t="s">
         <v>85</v>
-      </c>
-      <c r="P6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>86</v>
-      </c>
-      <c r="R6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S6" t="s">
-        <v>87</v>
-      </c>
-      <c r="T6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U6" t="s">
-        <v>88</v>
-      </c>
-      <c r="W6" t="s">
-        <v>39</v>
       </c>
       <c r="X6" t="s">
         <v>40</v>
       </c>
       <c r="Y6" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>90</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:27">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
         <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="H7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" t="s">
+        <v>90</v>
+      </c>
+      <c r="L7" t="s">
+        <v>91</v>
+      </c>
+      <c r="M7" t="s">
+        <v>92</v>
+      </c>
+      <c r="N7" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" t="s">
+        <v>93</v>
+      </c>
+      <c r="P7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" t="s">
         <v>94</v>
       </c>
-      <c r="I7" t="s">
+      <c r="R7" t="s">
+        <v>35</v>
+      </c>
+      <c r="S7" t="s">
         <v>95</v>
       </c>
-      <c r="L7" t="s">
+      <c r="T7" t="s">
+        <v>35</v>
+      </c>
+      <c r="U7" t="s">
         <v>96</v>
       </c>
-      <c r="M7" t="s">
-        <v>97</v>
-      </c>
-      <c r="N7" t="s">
-        <v>35</v>
-      </c>
-      <c r="O7" t="s">
-        <v>98</v>
-      </c>
-      <c r="P7" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>99</v>
-      </c>
-      <c r="R7" t="s">
-        <v>35</v>
-      </c>
-      <c r="S7" t="s">
-        <v>100</v>
-      </c>
-      <c r="T7" t="s">
-        <v>35</v>
-      </c>
-      <c r="U7" t="s">
-        <v>101</v>
-      </c>
       <c r="W7" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="X7" t="s">
         <v>40</v>
       </c>
       <c r="Y7" t="s">
-        <v>41</v>
+        <v>97</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:27">
       <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" t="s">
         <v>102</v>
       </c>
-      <c r="B8" t="s">
+      <c r="I8" t="s">
         <v>103</v>
       </c>
-      <c r="D8" t="s">
+      <c r="L8" t="s">
         <v>104</v>
       </c>
-      <c r="G8" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="M8" t="s">
         <v>105</v>
       </c>
-      <c r="I8" t="s">
+      <c r="N8" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" t="s">
         <v>106</v>
       </c>
-      <c r="L8" t="s">
+      <c r="P8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" t="s">
         <v>107</v>
       </c>
-      <c r="M8" t="s">
+      <c r="R8" t="s">
+        <v>35</v>
+      </c>
+      <c r="S8" t="s">
         <v>108</v>
       </c>
-      <c r="N8" t="s">
-        <v>35</v>
-      </c>
-      <c r="O8" t="s">
+      <c r="T8" t="s">
+        <v>35</v>
+      </c>
+      <c r="U8" t="s">
         <v>109</v>
       </c>
-      <c r="P8" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>110</v>
-      </c>
-      <c r="R8" t="s">
-        <v>35</v>
-      </c>
-      <c r="S8" t="s">
-        <v>111</v>
-      </c>
-      <c r="T8" t="s">
-        <v>35</v>
-      </c>
-      <c r="U8" t="s">
-        <v>112</v>
-      </c>
       <c r="W8" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="X8" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="Y8" t="s">
         <v>41</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:27">
       <c r="A9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9" t="s">
+        <v>113</v>
+      </c>
+      <c r="I9" t="s">
         <v>114</v>
       </c>
-      <c r="B9" t="s">
+      <c r="L9" t="s">
         <v>115</v>
       </c>
-      <c r="D9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G9" t="s">
-        <v>69</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="M9" t="s">
         <v>116</v>
       </c>
-      <c r="I9" t="s">
+      <c r="N9" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" t="s">
         <v>117</v>
       </c>
-      <c r="L9" t="s">
+      <c r="P9" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" t="s">
         <v>118</v>
       </c>
-      <c r="M9" t="s">
+      <c r="R9" t="s">
+        <v>35</v>
+      </c>
+      <c r="S9" t="s">
         <v>119</v>
       </c>
-      <c r="N9" t="s">
-        <v>35</v>
-      </c>
-      <c r="O9" t="s">
+      <c r="T9" t="s">
+        <v>35</v>
+      </c>
+      <c r="U9" t="s">
         <v>120</v>
       </c>
-      <c r="P9" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q9" t="s">
+      <c r="W9" t="s">
+        <v>85</v>
+      </c>
+      <c r="X9" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA9" t="s">
         <v>121</v>
-      </c>
-      <c r="R9" t="s">
-        <v>35</v>
-      </c>
-      <c r="S9" t="s">
-        <v>122</v>
-      </c>
-      <c r="T9" t="s">
-        <v>35</v>
-      </c>
-      <c r="U9" t="s">
-        <v>123</v>
-      </c>
-      <c r="W9" t="s">
-        <v>77</v>
-      </c>
-      <c r="X9" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:27">
       <c r="A10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" t="s">
         <v>124</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" t="s">
         <v>125</v>
       </c>
-      <c r="D10" t="s">
-        <v>104</v>
-      </c>
-      <c r="G10" t="s">
-        <v>69</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="L10" t="s">
         <v>126</v>
       </c>
-      <c r="I10" t="s">
+      <c r="M10" t="s">
         <v>127</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" t="s">
         <v>128</v>
       </c>
-      <c r="M10" t="s">
+      <c r="P10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q10" t="s">
         <v>129</v>
       </c>
-      <c r="N10" t="s">
-        <v>35</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="R10" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10" t="s">
         <v>130</v>
       </c>
-      <c r="P10" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>131</v>
-      </c>
-      <c r="R10" t="s">
-        <v>35</v>
-      </c>
-      <c r="S10" t="s">
-        <v>132</v>
-      </c>
       <c r="T10" t="s">
         <v>35</v>
       </c>
       <c r="W10" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="X10" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="Y10" t="s">
         <v>41</v>
@@ -2248,114 +2239,114 @@
     </row>
     <row r="11" spans="1:27">
       <c r="A11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" t="s">
+        <v>112</v>
+      </c>
+      <c r="G11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" t="s">
         <v>133</v>
       </c>
-      <c r="B11" t="s">
+      <c r="I11" t="s">
         <v>134</v>
       </c>
-      <c r="C11" t="s">
+      <c r="L11" t="s">
         <v>135</v>
       </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="M11" t="s">
         <v>136</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" t="s">
         <v>137</v>
       </c>
-      <c r="M11" t="s">
+      <c r="P11" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q11" t="s">
         <v>138</v>
       </c>
-      <c r="N11" t="s">
-        <v>35</v>
-      </c>
-      <c r="O11" t="s">
+      <c r="R11" t="s">
+        <v>35</v>
+      </c>
+      <c r="S11" t="s">
         <v>139</v>
       </c>
-      <c r="P11" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q11" t="s">
+      <c r="T11" t="s">
+        <v>35</v>
+      </c>
+      <c r="U11" t="s">
         <v>140</v>
       </c>
-      <c r="R11" t="s">
-        <v>35</v>
-      </c>
-      <c r="S11" t="s">
-        <v>141</v>
-      </c>
-      <c r="T11" t="s">
-        <v>35</v>
-      </c>
       <c r="W11" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="X11" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="Y11" t="s">
         <v>41</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:27">
       <c r="A12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" t="s">
+        <v>112</v>
+      </c>
+      <c r="G12" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" t="s">
         <v>143</v>
       </c>
-      <c r="B12" t="s">
+      <c r="I12" t="s">
         <v>144</v>
       </c>
-      <c r="D12" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="L12" t="s">
         <v>145</v>
       </c>
-      <c r="I12" t="s">
+      <c r="M12" t="s">
         <v>146</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
+        <v>35</v>
+      </c>
+      <c r="O12" t="s">
         <v>147</v>
       </c>
-      <c r="M12" t="s">
+      <c r="P12" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q12" t="s">
         <v>148</v>
       </c>
-      <c r="N12" t="s">
-        <v>35</v>
-      </c>
-      <c r="O12" t="s">
+      <c r="R12" t="s">
+        <v>35</v>
+      </c>
+      <c r="S12" t="s">
         <v>149</v>
       </c>
-      <c r="P12" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>150</v>
-      </c>
-      <c r="R12" t="s">
-        <v>35</v>
-      </c>
-      <c r="S12" t="s">
-        <v>151</v>
-      </c>
       <c r="T12" t="s">
         <v>35</v>
       </c>
       <c r="W12" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="X12" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="Y12" t="s">
         <v>41</v>
@@ -2363,52 +2354,52 @@
     </row>
     <row r="13" spans="1:27">
       <c r="A13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" t="s">
         <v>152</v>
       </c>
-      <c r="B13" t="s">
-        <v>153</v>
-      </c>
       <c r="D13" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="G13" t="s">
         <v>30</v>
       </c>
       <c r="H13" t="s">
+        <v>153</v>
+      </c>
+      <c r="I13" t="s">
         <v>154</v>
       </c>
-      <c r="I13" t="s">
+      <c r="L13" t="s">
         <v>155</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>156</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" t="s">
         <v>157</v>
       </c>
-      <c r="N13" t="s">
-        <v>35</v>
-      </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q13" t="s">
         <v>158</v>
       </c>
-      <c r="P13" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
+        <v>35</v>
+      </c>
+      <c r="S13" t="s">
         <v>159</v>
       </c>
-      <c r="R13" t="s">
-        <v>35</v>
-      </c>
-      <c r="S13" t="s">
-        <v>160</v>
-      </c>
       <c r="T13" t="s">
         <v>35</v>
-      </c>
-      <c r="U13" t="s">
-        <v>161</v>
       </c>
       <c r="W13" t="s">
         <v>39</v>
@@ -2419,49 +2410,52 @@
       <c r="Y13" t="s">
         <v>41</v>
       </c>
+      <c r="AA13" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="14" spans="1:27">
       <c r="A14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" t="s">
         <v>162</v>
       </c>
-      <c r="B14" t="s">
-        <v>163</v>
-      </c>
-      <c r="C14" t="s">
-        <v>164</v>
-      </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>112</v>
       </c>
       <c r="G14" t="s">
         <v>45</v>
       </c>
+      <c r="H14" t="s">
+        <v>163</v>
+      </c>
       <c r="I14" t="s">
+        <v>164</v>
+      </c>
+      <c r="L14" t="s">
         <v>165</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>166</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" t="s">
         <v>167</v>
       </c>
-      <c r="N14" t="s">
-        <v>35</v>
-      </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q14" t="s">
         <v>168</v>
       </c>
-      <c r="P14" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
+        <v>35</v>
+      </c>
+      <c r="S14" t="s">
         <v>169</v>
-      </c>
-      <c r="R14" t="s">
-        <v>35</v>
-      </c>
-      <c r="S14" t="s">
-        <v>170</v>
       </c>
       <c r="T14" t="s">
         <v>35</v>
@@ -2478,55 +2472,58 @@
     </row>
     <row r="15" spans="1:27">
       <c r="A15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" t="s">
         <v>171</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" t="s">
         <v>172</v>
       </c>
-      <c r="D15" t="s">
-        <v>104</v>
-      </c>
-      <c r="G15" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>173</v>
       </c>
-      <c r="I15" t="s">
+      <c r="L15" t="s">
         <v>174</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>175</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
+        <v>35</v>
+      </c>
+      <c r="O15" t="s">
         <v>176</v>
       </c>
-      <c r="N15" t="s">
-        <v>35</v>
-      </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q15" t="s">
         <v>177</v>
       </c>
-      <c r="P15" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
+        <v>35</v>
+      </c>
+      <c r="S15" t="s">
         <v>178</v>
       </c>
-      <c r="R15" t="s">
-        <v>35</v>
-      </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
+        <v>35</v>
+      </c>
+      <c r="U15" t="s">
         <v>179</v>
       </c>
-      <c r="T15" t="s">
-        <v>35</v>
-      </c>
       <c r="W15" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="X15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Y15" t="s">
         <v>41</v>
@@ -2539,14 +2536,14 @@
       <c r="B16" t="s">
         <v>181</v>
       </c>
+      <c r="C16" t="s">
+        <v>182</v>
+      </c>
       <c r="D16" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" t="s">
-        <v>182</v>
+        <v>45</v>
       </c>
       <c r="I16" t="s">
         <v>183</v>
@@ -2582,35 +2579,35 @@
         <v>189</v>
       </c>
       <c r="W16" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="X16" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="Y16" t="s">
         <v>41</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:27">
       <c r="A17" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B17" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D17" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="G17" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H17" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I17" t="s">
-        <v>193</v>
-      </c>
-      <c r="J17" t="s">
         <v>194</v>
       </c>
       <c r="L17" t="s">
@@ -2640,114 +2637,279 @@
       <c r="T17" t="s">
         <v>35</v>
       </c>
-      <c r="U17" t="s">
+      <c r="W17" t="s">
+        <v>39</v>
+      </c>
+      <c r="X17" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA17" t="s">
         <v>200</v>
       </c>
-      <c r="W17" t="s">
+    </row>
+    <row r="18" spans="1:27">
+      <c r="A18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18" t="s">
+        <v>112</v>
+      </c>
+      <c r="G18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" t="s">
+        <v>154</v>
+      </c>
+      <c r="L18" t="s">
+        <v>203</v>
+      </c>
+      <c r="M18" t="s">
+        <v>204</v>
+      </c>
+      <c r="N18" t="s">
+        <v>35</v>
+      </c>
+      <c r="O18" t="s">
+        <v>205</v>
+      </c>
+      <c r="P18" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>206</v>
+      </c>
+      <c r="R18" t="s">
+        <v>35</v>
+      </c>
+      <c r="S18" t="s">
+        <v>207</v>
+      </c>
+      <c r="T18" t="s">
+        <v>35</v>
+      </c>
+      <c r="W18" t="s">
+        <v>85</v>
+      </c>
+      <c r="X18" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27">
+      <c r="A19" t="s">
+        <v>208</v>
+      </c>
+      <c r="B19" t="s">
+        <v>209</v>
+      </c>
+      <c r="D19" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" t="s">
+        <v>210</v>
+      </c>
+      <c r="I19" t="s">
+        <v>211</v>
+      </c>
+      <c r="L19" t="s">
+        <v>212</v>
+      </c>
+      <c r="M19" t="s">
+        <v>213</v>
+      </c>
+      <c r="N19" t="s">
+        <v>35</v>
+      </c>
+      <c r="O19" t="s">
+        <v>214</v>
+      </c>
+      <c r="P19" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>215</v>
+      </c>
+      <c r="R19" t="s">
+        <v>35</v>
+      </c>
+      <c r="S19" t="s">
+        <v>216</v>
+      </c>
+      <c r="T19" t="s">
+        <v>35</v>
+      </c>
+      <c r="U19" t="s">
+        <v>217</v>
+      </c>
+      <c r="W19" t="s">
+        <v>85</v>
+      </c>
+      <c r="X19" t="s">
         <v>65</v>
       </c>
-      <c r="X17" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>201</v>
+      <c r="Y19" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:27">
       <c r="A20" t="s">
-        <v>202</v>
-      </c>
-      <c r="C20" t="s">
-        <v>203</v>
+        <v>218</v>
+      </c>
+      <c r="B20" t="s">
+        <v>219</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>112</v>
+      </c>
+      <c r="G20" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" t="s">
+        <v>220</v>
       </c>
       <c r="I20" t="s">
-        <v>204</v>
+        <v>221</v>
+      </c>
+      <c r="L20" t="s">
+        <v>222</v>
+      </c>
+      <c r="M20" t="s">
+        <v>223</v>
+      </c>
+      <c r="N20" t="s">
+        <v>35</v>
+      </c>
+      <c r="O20" t="s">
+        <v>224</v>
+      </c>
+      <c r="P20" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>225</v>
+      </c>
+      <c r="R20" t="s">
+        <v>35</v>
+      </c>
+      <c r="S20" t="s">
+        <v>226</v>
+      </c>
+      <c r="T20" t="s">
+        <v>35</v>
+      </c>
+      <c r="U20" t="s">
+        <v>227</v>
+      </c>
+      <c r="W20" t="s">
+        <v>85</v>
+      </c>
+      <c r="X20" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:27">
       <c r="A21" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="B21" t="s">
-        <v>206</v>
-      </c>
-      <c r="C21" t="s">
-        <v>207</v>
+        <v>229</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>112</v>
+      </c>
+      <c r="G21" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" t="s">
+        <v>230</v>
       </c>
       <c r="I21" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27">
-      <c r="A22" t="s">
-        <v>209</v>
-      </c>
-      <c r="B22" t="s">
-        <v>210</v>
-      </c>
-      <c r="D22" t="s">
-        <v>104</v>
-      </c>
-      <c r="G22" t="s">
-        <v>211</v>
-      </c>
-      <c r="H22" t="s">
-        <v>212</v>
-      </c>
-      <c r="I22" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27">
-      <c r="A23" t="s">
-        <v>214</v>
-      </c>
-      <c r="B23" t="s">
-        <v>215</v>
-      </c>
-      <c r="D23" t="s">
-        <v>104</v>
-      </c>
-      <c r="G23" t="s">
-        <v>216</v>
+        <v>231</v>
+      </c>
+      <c r="J21" t="s">
+        <v>232</v>
+      </c>
+      <c r="L21" t="s">
+        <v>233</v>
+      </c>
+      <c r="M21" t="s">
+        <v>234</v>
+      </c>
+      <c r="N21" t="s">
+        <v>35</v>
+      </c>
+      <c r="O21" t="s">
+        <v>235</v>
+      </c>
+      <c r="P21" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>236</v>
+      </c>
+      <c r="R21" t="s">
+        <v>35</v>
+      </c>
+      <c r="S21" t="s">
+        <v>237</v>
+      </c>
+      <c r="T21" t="s">
+        <v>35</v>
+      </c>
+      <c r="W21" t="s">
+        <v>53</v>
+      </c>
+      <c r="X21" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:27">
       <c r="L26" t="s">
-        <v>217</v>
+        <v>238</v>
       </c>
       <c r="M26" t="s">
-        <v>218</v>
+        <v>239</v>
       </c>
       <c r="N26" t="s">
         <v>35</v>
       </c>
       <c r="O26" t="s">
-        <v>219</v>
+        <v>240</v>
       </c>
       <c r="P26" t="s">
         <v>35</v>
       </c>
       <c r="Q26" t="s">
-        <v>220</v>
+        <v>241</v>
       </c>
       <c r="R26" t="s">
         <v>35</v>
       </c>
       <c r="S26" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="T26" t="s">
         <v>35</v>
+      </c>
+      <c r="U26" t="s">
+        <v>243</v>
       </c>
       <c r="W26" t="s">
         <v>39</v>
@@ -2759,42 +2921,80 @@
         <v>41</v>
       </c>
       <c r="AA26" t="s">
-        <v>222</v>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27">
+      <c r="L27" t="s">
+        <v>245</v>
+      </c>
+      <c r="M27" t="s">
+        <v>246</v>
+      </c>
+      <c r="N27" t="s">
+        <v>35</v>
+      </c>
+      <c r="O27" t="s">
+        <v>247</v>
+      </c>
+      <c r="P27" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>248</v>
+      </c>
+      <c r="R27" t="s">
+        <v>35</v>
+      </c>
+      <c r="S27" t="s">
+        <v>249</v>
+      </c>
+      <c r="T27" t="s">
+        <v>35</v>
+      </c>
+      <c r="U27" t="s">
+        <v>250</v>
+      </c>
+      <c r="W27" t="s">
+        <v>65</v>
+      </c>
+      <c r="X27" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:27">
       <c r="L28" t="s">
-        <v>223</v>
+        <v>251</v>
       </c>
       <c r="M28" t="s">
-        <v>224</v>
+        <v>252</v>
       </c>
       <c r="N28" t="s">
         <v>35</v>
       </c>
       <c r="O28" t="s">
-        <v>225</v>
+        <v>253</v>
       </c>
       <c r="P28" t="s">
         <v>35</v>
       </c>
       <c r="Q28" t="s">
-        <v>226</v>
+        <v>254</v>
       </c>
       <c r="R28" t="s">
         <v>35</v>
       </c>
       <c r="S28" t="s">
-        <v>227</v>
+        <v>255</v>
       </c>
       <c r="T28" t="s">
         <v>35</v>
       </c>
-      <c r="U28" t="s">
-        <v>228</v>
-      </c>
       <c r="W28" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="X28" t="s">
         <v>40</v>
@@ -2803,36 +3003,83 @@
         <v>41</v>
       </c>
       <c r="AA28" t="s">
-        <v>229</v>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27">
+      <c r="L29" t="s">
+        <v>257</v>
+      </c>
+      <c r="M29" t="s">
+        <v>258</v>
+      </c>
+      <c r="N29" t="s">
+        <v>35</v>
+      </c>
+      <c r="O29" t="s">
+        <v>259</v>
+      </c>
+      <c r="P29" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>260</v>
+      </c>
+      <c r="R29" t="s">
+        <v>35</v>
+      </c>
+      <c r="S29" t="s">
+        <v>261</v>
+      </c>
+      <c r="T29" t="s">
+        <v>35</v>
+      </c>
+      <c r="U29" t="s">
+        <v>262</v>
+      </c>
+      <c r="W29" t="s">
+        <v>65</v>
+      </c>
+      <c r="X29" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:27">
       <c r="L30" t="s">
-        <v>230</v>
+        <v>264</v>
       </c>
       <c r="M30" t="s">
-        <v>231</v>
+        <v>265</v>
       </c>
       <c r="N30" t="s">
         <v>35</v>
       </c>
       <c r="O30" t="s">
-        <v>232</v>
+        <v>266</v>
       </c>
       <c r="P30" t="s">
         <v>35</v>
       </c>
       <c r="Q30" t="s">
-        <v>233</v>
+        <v>267</v>
       </c>
       <c r="R30" t="s">
         <v>35</v>
       </c>
       <c r="S30" t="s">
-        <v>234</v>
+        <v>268</v>
       </c>
       <c r="T30" t="s">
         <v>35</v>
+      </c>
+      <c r="U30" t="s">
+        <v>269</v>
       </c>
       <c r="W30" t="s">
         <v>65</v>
@@ -2844,443 +3091,879 @@
         <v>41</v>
       </c>
     </row>
+    <row r="31" spans="1:27">
+      <c r="L31" t="s">
+        <v>270</v>
+      </c>
+      <c r="M31" t="s">
+        <v>271</v>
+      </c>
+      <c r="N31" t="s">
+        <v>35</v>
+      </c>
+      <c r="O31" t="s">
+        <v>272</v>
+      </c>
+      <c r="P31" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>273</v>
+      </c>
+      <c r="R31" t="s">
+        <v>35</v>
+      </c>
+      <c r="S31" t="s">
+        <v>274</v>
+      </c>
+      <c r="T31" t="s">
+        <v>35</v>
+      </c>
+      <c r="W31" t="s">
+        <v>85</v>
+      </c>
+      <c r="X31" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="32" spans="1:27">
       <c r="L32" t="s">
-        <v>235</v>
+        <v>275</v>
       </c>
       <c r="M32" t="s">
-        <v>236</v>
+        <v>276</v>
       </c>
       <c r="N32" t="s">
         <v>35</v>
       </c>
       <c r="O32" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="P32" t="s">
         <v>35</v>
       </c>
       <c r="Q32" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
       <c r="R32" t="s">
         <v>35</v>
       </c>
       <c r="S32" t="s">
-        <v>239</v>
+        <v>279</v>
       </c>
       <c r="T32" t="s">
         <v>35</v>
       </c>
       <c r="U32" t="s">
-        <v>240</v>
+        <v>280</v>
       </c>
       <c r="W32" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="X32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Y32" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="33" spans="12:27">
+      <c r="L33" t="s">
+        <v>282</v>
+      </c>
+      <c r="M33" t="s">
+        <v>283</v>
+      </c>
+      <c r="N33" t="s">
+        <v>35</v>
+      </c>
+      <c r="O33" t="s">
+        <v>284</v>
+      </c>
+      <c r="P33" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>285</v>
+      </c>
+      <c r="R33" t="s">
+        <v>35</v>
+      </c>
+      <c r="S33" t="s">
+        <v>286</v>
+      </c>
+      <c r="T33" t="s">
+        <v>35</v>
+      </c>
+      <c r="W33" t="s">
+        <v>85</v>
+      </c>
+      <c r="X33" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="34" spans="12:27">
       <c r="L34" t="s">
-        <v>241</v>
+        <v>287</v>
       </c>
       <c r="M34" t="s">
-        <v>242</v>
+        <v>288</v>
       </c>
       <c r="N34" t="s">
         <v>35</v>
       </c>
       <c r="O34" t="s">
-        <v>243</v>
+        <v>289</v>
       </c>
       <c r="P34" t="s">
         <v>35</v>
       </c>
       <c r="Q34" t="s">
-        <v>244</v>
+        <v>290</v>
       </c>
       <c r="R34" t="s">
         <v>35</v>
       </c>
       <c r="S34" t="s">
-        <v>245</v>
+        <v>291</v>
       </c>
       <c r="T34" t="s">
         <v>35</v>
       </c>
+      <c r="U34" t="s">
+        <v>292</v>
+      </c>
       <c r="W34" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="X34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Y34" t="s">
         <v>41</v>
       </c>
-      <c r="AA34" t="s">
-        <v>246</v>
+    </row>
+    <row r="35" spans="12:27">
+      <c r="L35" t="s">
+        <v>293</v>
+      </c>
+      <c r="M35" t="s">
+        <v>294</v>
+      </c>
+      <c r="N35" t="s">
+        <v>35</v>
+      </c>
+      <c r="O35" t="s">
+        <v>295</v>
+      </c>
+      <c r="P35" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>296</v>
+      </c>
+      <c r="R35" t="s">
+        <v>35</v>
+      </c>
+      <c r="S35" t="s">
+        <v>297</v>
+      </c>
+      <c r="T35" t="s">
+        <v>35</v>
+      </c>
+      <c r="W35" t="s">
+        <v>85</v>
+      </c>
+      <c r="X35" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="12:27">
       <c r="L36" t="s">
-        <v>247</v>
+        <v>298</v>
       </c>
       <c r="M36" t="s">
-        <v>248</v>
+        <v>299</v>
       </c>
       <c r="N36" t="s">
         <v>35</v>
       </c>
       <c r="O36" t="s">
-        <v>249</v>
+        <v>300</v>
       </c>
       <c r="P36" t="s">
         <v>35</v>
       </c>
       <c r="Q36" t="s">
-        <v>250</v>
+        <v>301</v>
       </c>
       <c r="R36" t="s">
         <v>35</v>
       </c>
       <c r="S36" t="s">
-        <v>251</v>
+        <v>302</v>
       </c>
       <c r="T36" t="s">
         <v>35</v>
       </c>
-      <c r="U36" t="s">
-        <v>252</v>
-      </c>
       <c r="W36" t="s">
+        <v>85</v>
+      </c>
+      <c r="X36" t="s">
         <v>65</v>
       </c>
-      <c r="X36" t="s">
-        <v>40</v>
-      </c>
       <c r="Y36" t="s">
         <v>41</v>
       </c>
-      <c r="AA36" t="s">
-        <v>253</v>
+    </row>
+    <row r="37" spans="12:27">
+      <c r="L37" t="s">
+        <v>303</v>
+      </c>
+      <c r="M37" t="s">
+        <v>304</v>
+      </c>
+      <c r="N37" t="s">
+        <v>35</v>
+      </c>
+      <c r="O37" t="s">
+        <v>305</v>
+      </c>
+      <c r="P37" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>306</v>
+      </c>
+      <c r="R37" t="s">
+        <v>35</v>
+      </c>
+      <c r="S37" t="s">
+        <v>307</v>
+      </c>
+      <c r="T37" t="s">
+        <v>35</v>
+      </c>
+      <c r="U37" t="s">
+        <v>308</v>
+      </c>
+      <c r="W37" t="s">
+        <v>85</v>
+      </c>
+      <c r="X37" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="12:27">
       <c r="L38" t="s">
-        <v>254</v>
+        <v>309</v>
       </c>
       <c r="M38" t="s">
-        <v>255</v>
+        <v>310</v>
       </c>
       <c r="N38" t="s">
         <v>35</v>
       </c>
       <c r="O38" t="s">
-        <v>256</v>
+        <v>311</v>
       </c>
       <c r="P38" t="s">
         <v>35</v>
       </c>
       <c r="Q38" t="s">
-        <v>257</v>
+        <v>312</v>
       </c>
       <c r="R38" t="s">
         <v>35</v>
       </c>
       <c r="S38" t="s">
-        <v>258</v>
+        <v>313</v>
       </c>
       <c r="T38" t="s">
         <v>35</v>
       </c>
-      <c r="U38" t="s">
-        <v>259</v>
-      </c>
       <c r="W38" t="s">
+        <v>85</v>
+      </c>
+      <c r="X38" t="s">
         <v>65</v>
       </c>
-      <c r="X38" t="s">
-        <v>40</v>
-      </c>
       <c r="Y38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="12:27">
+      <c r="L39" t="s">
+        <v>314</v>
+      </c>
+      <c r="M39" t="s">
+        <v>315</v>
+      </c>
+      <c r="N39" t="s">
+        <v>35</v>
+      </c>
+      <c r="O39" t="s">
+        <v>316</v>
+      </c>
+      <c r="P39" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>317</v>
+      </c>
+      <c r="R39" t="s">
+        <v>35</v>
+      </c>
+      <c r="S39" t="s">
+        <v>318</v>
+      </c>
+      <c r="T39" t="s">
+        <v>35</v>
+      </c>
+      <c r="U39" t="s">
+        <v>319</v>
+      </c>
+      <c r="W39" t="s">
+        <v>85</v>
+      </c>
+      <c r="X39" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y39" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="40" spans="12:27">
       <c r="L40" t="s">
-        <v>260</v>
+        <v>320</v>
       </c>
       <c r="M40" t="s">
-        <v>261</v>
+        <v>321</v>
       </c>
       <c r="N40" t="s">
         <v>35</v>
       </c>
       <c r="O40" t="s">
-        <v>262</v>
+        <v>322</v>
       </c>
       <c r="P40" t="s">
         <v>35</v>
       </c>
       <c r="Q40" t="s">
-        <v>263</v>
+        <v>323</v>
       </c>
       <c r="R40" t="s">
         <v>35</v>
       </c>
       <c r="S40" t="s">
-        <v>264</v>
+        <v>324</v>
       </c>
       <c r="T40" t="s">
         <v>35</v>
       </c>
-      <c r="U40" t="s">
-        <v>265</v>
-      </c>
       <c r="W40" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="X40" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="Y40" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="12:27">
+      <c r="L41" t="s">
+        <v>325</v>
+      </c>
+      <c r="M41" t="s">
+        <v>326</v>
+      </c>
+      <c r="N41" t="s">
+        <v>35</v>
+      </c>
+      <c r="O41" t="s">
+        <v>327</v>
+      </c>
+      <c r="P41" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>328</v>
+      </c>
+      <c r="R41" t="s">
+        <v>35</v>
+      </c>
+      <c r="S41" t="s">
+        <v>329</v>
+      </c>
+      <c r="T41" t="s">
+        <v>35</v>
+      </c>
+      <c r="U41" t="s">
+        <v>330</v>
+      </c>
+      <c r="W41" t="s">
+        <v>85</v>
+      </c>
+      <c r="X41" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="42" spans="12:27">
       <c r="L42" t="s">
-        <v>266</v>
+        <v>332</v>
       </c>
       <c r="M42" t="s">
-        <v>267</v>
+        <v>333</v>
       </c>
       <c r="N42" t="s">
         <v>35</v>
       </c>
       <c r="O42" t="s">
-        <v>268</v>
+        <v>334</v>
       </c>
       <c r="P42" t="s">
         <v>35</v>
       </c>
       <c r="Q42" t="s">
-        <v>269</v>
+        <v>335</v>
       </c>
       <c r="R42" t="s">
         <v>35</v>
       </c>
       <c r="S42" t="s">
-        <v>270</v>
+        <v>336</v>
       </c>
       <c r="T42" t="s">
         <v>35</v>
       </c>
       <c r="W42" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="X42" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="Y42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="12:27">
+      <c r="L43" t="s">
+        <v>337</v>
+      </c>
+      <c r="M43" t="s">
+        <v>338</v>
+      </c>
+      <c r="N43" t="s">
+        <v>35</v>
+      </c>
+      <c r="O43" t="s">
+        <v>339</v>
+      </c>
+      <c r="P43" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>340</v>
+      </c>
+      <c r="R43" t="s">
+        <v>35</v>
+      </c>
+      <c r="S43" t="s">
+        <v>341</v>
+      </c>
+      <c r="T43" t="s">
+        <v>35</v>
+      </c>
+      <c r="U43" t="s">
+        <v>342</v>
+      </c>
+      <c r="W43" t="s">
+        <v>53</v>
+      </c>
+      <c r="X43" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y43" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="44" spans="12:27">
       <c r="L44" t="s">
-        <v>271</v>
+        <v>343</v>
       </c>
       <c r="M44" t="s">
-        <v>272</v>
+        <v>344</v>
       </c>
       <c r="N44" t="s">
         <v>35</v>
       </c>
       <c r="O44" t="s">
-        <v>273</v>
+        <v>345</v>
       </c>
       <c r="P44" t="s">
         <v>35</v>
       </c>
       <c r="Q44" t="s">
-        <v>274</v>
+        <v>346</v>
       </c>
       <c r="R44" t="s">
         <v>35</v>
       </c>
       <c r="S44" t="s">
-        <v>275</v>
+        <v>347</v>
       </c>
       <c r="T44" t="s">
         <v>35</v>
       </c>
-      <c r="U44" t="s">
-        <v>276</v>
-      </c>
       <c r="W44" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="X44" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="Y44" t="s">
         <v>41</v>
       </c>
-      <c r="AA44" t="s">
-        <v>277</v>
+    </row>
+    <row r="45" spans="12:27">
+      <c r="L45" t="s">
+        <v>348</v>
+      </c>
+      <c r="M45" t="s">
+        <v>349</v>
+      </c>
+      <c r="N45" t="s">
+        <v>35</v>
+      </c>
+      <c r="O45" t="s">
+        <v>350</v>
+      </c>
+      <c r="P45" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>351</v>
+      </c>
+      <c r="R45" t="s">
+        <v>35</v>
+      </c>
+      <c r="S45" t="s">
+        <v>352</v>
+      </c>
+      <c r="T45" t="s">
+        <v>35</v>
+      </c>
+      <c r="U45" t="s">
+        <v>353</v>
+      </c>
+      <c r="W45" t="s">
+        <v>53</v>
+      </c>
+      <c r="X45" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="12:27">
       <c r="L46" t="s">
-        <v>278</v>
+        <v>354</v>
       </c>
       <c r="M46" t="s">
-        <v>279</v>
+        <v>355</v>
       </c>
       <c r="N46" t="s">
         <v>35</v>
       </c>
       <c r="O46" t="s">
-        <v>280</v>
+        <v>356</v>
       </c>
       <c r="P46" t="s">
         <v>35</v>
       </c>
       <c r="Q46" t="s">
-        <v>281</v>
+        <v>357</v>
       </c>
       <c r="R46" t="s">
         <v>35</v>
       </c>
       <c r="S46" t="s">
-        <v>282</v>
+        <v>358</v>
       </c>
       <c r="T46" t="s">
         <v>35</v>
       </c>
+      <c r="U46" t="s">
+        <v>359</v>
+      </c>
       <c r="W46" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="X46" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="12:27">
+      <c r="L47" t="s">
+        <v>360</v>
+      </c>
+      <c r="M47" t="s">
+        <v>361</v>
+      </c>
+      <c r="N47" t="s">
+        <v>35</v>
+      </c>
+      <c r="O47" t="s">
+        <v>362</v>
+      </c>
+      <c r="P47" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>363</v>
+      </c>
+      <c r="R47" t="s">
+        <v>35</v>
+      </c>
+      <c r="S47" t="s">
+        <v>364</v>
+      </c>
+      <c r="T47" t="s">
+        <v>35</v>
+      </c>
+      <c r="U47" t="s">
+        <v>365</v>
+      </c>
+      <c r="W47" t="s">
         <v>39</v>
       </c>
-      <c r="Y46" t="s">
+      <c r="X47" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y47" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="48" spans="12:27">
       <c r="L48" t="s">
-        <v>283</v>
+        <v>366</v>
       </c>
       <c r="M48" t="s">
-        <v>284</v>
+        <v>367</v>
       </c>
       <c r="N48" t="s">
         <v>35</v>
       </c>
       <c r="O48" t="s">
-        <v>285</v>
+        <v>368</v>
       </c>
       <c r="P48" t="s">
         <v>35</v>
       </c>
       <c r="Q48" t="s">
-        <v>286</v>
+        <v>369</v>
       </c>
       <c r="R48" t="s">
         <v>35</v>
       </c>
       <c r="S48" t="s">
-        <v>287</v>
+        <v>370</v>
       </c>
       <c r="T48" t="s">
         <v>35</v>
       </c>
       <c r="U48" t="s">
-        <v>288</v>
+        <v>371</v>
       </c>
       <c r="W48" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="X48" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="Y48" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="12:27">
+    <row r="49" spans="12:25">
+      <c r="L49" t="s">
+        <v>372</v>
+      </c>
+      <c r="M49" t="s">
+        <v>373</v>
+      </c>
+      <c r="N49" t="s">
+        <v>35</v>
+      </c>
+      <c r="O49" t="s">
+        <v>374</v>
+      </c>
+      <c r="P49" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>375</v>
+      </c>
+      <c r="R49" t="s">
+        <v>35</v>
+      </c>
+      <c r="S49" t="s">
+        <v>376</v>
+      </c>
+      <c r="T49" t="s">
+        <v>35</v>
+      </c>
+      <c r="W49" t="s">
+        <v>53</v>
+      </c>
+      <c r="X49" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="12:25">
       <c r="L50" t="s">
-        <v>289</v>
+        <v>377</v>
       </c>
       <c r="M50" t="s">
-        <v>290</v>
+        <v>378</v>
       </c>
       <c r="N50" t="s">
         <v>35</v>
       </c>
       <c r="O50" t="s">
-        <v>291</v>
+        <v>379</v>
       </c>
       <c r="P50" t="s">
         <v>35</v>
       </c>
       <c r="Q50" t="s">
+        <v>380</v>
+      </c>
+      <c r="R50" t="s">
+        <v>35</v>
+      </c>
+      <c r="S50" t="s">
+        <v>381</v>
+      </c>
+      <c r="T50" t="s">
+        <v>35</v>
+      </c>
+      <c r="U50" t="s">
+        <v>382</v>
+      </c>
+      <c r="W50" t="s">
+        <v>65</v>
+      </c>
+      <c r="X50" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="12:25">
+      <c r="L51" t="s">
+        <v>383</v>
+      </c>
+      <c r="M51" t="s">
+        <v>384</v>
+      </c>
+      <c r="N51" t="s">
+        <v>35</v>
+      </c>
+      <c r="O51" t="s">
+        <v>385</v>
+      </c>
+      <c r="P51" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>386</v>
+      </c>
+      <c r="R51" t="s">
+        <v>35</v>
+      </c>
+      <c r="S51" t="s">
+        <v>387</v>
+      </c>
+      <c r="T51" t="s">
+        <v>35</v>
+      </c>
+      <c r="U51" t="s">
+        <v>388</v>
+      </c>
+      <c r="W51" t="s">
+        <v>65</v>
+      </c>
+      <c r="X51" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="12:25">
+      <c r="L52" t="s">
+        <v>389</v>
+      </c>
+      <c r="M52" t="s">
+        <v>390</v>
+      </c>
+      <c r="N52" t="s">
+        <v>35</v>
+      </c>
+      <c r="O52" t="s">
+        <v>391</v>
+      </c>
+      <c r="P52" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>392</v>
+      </c>
+      <c r="R52" t="s">
+        <v>35</v>
+      </c>
+      <c r="S52" t="s">
+        <v>393</v>
+      </c>
+      <c r="T52" t="s">
+        <v>35</v>
+      </c>
+      <c r="U52" t="s">
         <v>292</v>
       </c>
-      <c r="R50" t="s">
-        <v>35</v>
-      </c>
-      <c r="S50" t="s">
-        <v>293</v>
-      </c>
-      <c r="T50" t="s">
-        <v>35</v>
-      </c>
-      <c r="W50" t="s">
-        <v>77</v>
-      </c>
-      <c r="X50" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y50" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="52" spans="12:27">
-      <c r="L52" t="s">
-        <v>294</v>
-      </c>
-      <c r="M52" t="s">
-        <v>295</v>
-      </c>
-      <c r="N52" t="s">
-        <v>35</v>
-      </c>
-      <c r="O52" t="s">
-        <v>296</v>
-      </c>
-      <c r="P52" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q52" t="s">
-        <v>297</v>
-      </c>
-      <c r="R52" t="s">
-        <v>35</v>
-      </c>
-      <c r="S52" t="s">
-        <v>298</v>
-      </c>
-      <c r="T52" t="s">
-        <v>35</v>
-      </c>
       <c r="W52" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="X52" t="s">
         <v>65</v>
@@ -3289,39 +3972,80 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="12:27">
+    <row r="53" spans="12:25">
+      <c r="L53" t="s">
+        <v>394</v>
+      </c>
+      <c r="M53" t="s">
+        <v>395</v>
+      </c>
+      <c r="N53" t="s">
+        <v>35</v>
+      </c>
+      <c r="O53" t="s">
+        <v>396</v>
+      </c>
+      <c r="P53" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>397</v>
+      </c>
+      <c r="R53" t="s">
+        <v>35</v>
+      </c>
+      <c r="S53" t="s">
+        <v>398</v>
+      </c>
+      <c r="T53" t="s">
+        <v>35</v>
+      </c>
+      <c r="U53" t="s">
+        <v>399</v>
+      </c>
+      <c r="W53" t="s">
+        <v>53</v>
+      </c>
+      <c r="X53" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="12:25">
       <c r="L54" t="s">
-        <v>299</v>
+        <v>400</v>
       </c>
       <c r="M54" t="s">
-        <v>300</v>
+        <v>401</v>
       </c>
       <c r="N54" t="s">
         <v>35</v>
       </c>
       <c r="O54" t="s">
-        <v>301</v>
+        <v>402</v>
       </c>
       <c r="P54" t="s">
         <v>35</v>
       </c>
       <c r="Q54" t="s">
-        <v>302</v>
+        <v>403</v>
       </c>
       <c r="R54" t="s">
         <v>35</v>
       </c>
       <c r="S54" t="s">
-        <v>303</v>
+        <v>404</v>
       </c>
       <c r="T54" t="s">
         <v>35</v>
       </c>
       <c r="U54" t="s">
-        <v>304</v>
+        <v>405</v>
       </c>
       <c r="W54" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="X54" t="s">
         <v>65</v>
@@ -3330,36 +4054,80 @@
         <v>41</v>
       </c>
     </row>
-    <row r="56" spans="12:27">
+    <row r="55" spans="12:25">
+      <c r="L55" t="s">
+        <v>406</v>
+      </c>
+      <c r="M55" t="s">
+        <v>407</v>
+      </c>
+      <c r="N55" t="s">
+        <v>35</v>
+      </c>
+      <c r="O55" t="s">
+        <v>408</v>
+      </c>
+      <c r="P55" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>409</v>
+      </c>
+      <c r="R55" t="s">
+        <v>35</v>
+      </c>
+      <c r="S55" t="s">
+        <v>410</v>
+      </c>
+      <c r="T55" t="s">
+        <v>35</v>
+      </c>
+      <c r="U55" t="s">
+        <v>411</v>
+      </c>
+      <c r="W55" t="s">
+        <v>53</v>
+      </c>
+      <c r="X55" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="12:25">
       <c r="L56" t="s">
-        <v>305</v>
+        <v>412</v>
       </c>
       <c r="M56" t="s">
-        <v>306</v>
+        <v>413</v>
       </c>
       <c r="N56" t="s">
         <v>35</v>
       </c>
       <c r="O56" t="s">
-        <v>307</v>
+        <v>414</v>
       </c>
       <c r="P56" t="s">
         <v>35</v>
       </c>
       <c r="Q56" t="s">
-        <v>308</v>
+        <v>415</v>
       </c>
       <c r="R56" t="s">
         <v>35</v>
       </c>
       <c r="S56" t="s">
-        <v>309</v>
+        <v>416</v>
       </c>
       <c r="T56" t="s">
         <v>35</v>
       </c>
+      <c r="U56" t="s">
+        <v>417</v>
+      </c>
       <c r="W56" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="X56" t="s">
         <v>65</v>
@@ -3368,811 +4136,44 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="12:27">
-      <c r="L58" t="s">
-        <v>310</v>
-      </c>
-      <c r="M58" t="s">
-        <v>311</v>
-      </c>
-      <c r="N58" t="s">
-        <v>35</v>
-      </c>
-      <c r="O58" t="s">
-        <v>312</v>
-      </c>
-      <c r="P58" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>313</v>
-      </c>
-      <c r="R58" t="s">
-        <v>35</v>
-      </c>
-      <c r="S58" t="s">
-        <v>314</v>
-      </c>
-      <c r="T58" t="s">
-        <v>35</v>
-      </c>
-      <c r="U58" t="s">
-        <v>315</v>
-      </c>
-      <c r="W58" t="s">
-        <v>77</v>
-      </c>
-      <c r="X58" t="s">
+    <row r="57" spans="12:25">
+      <c r="L57" t="s">
+        <v>418</v>
+      </c>
+      <c r="M57" t="s">
+        <v>419</v>
+      </c>
+      <c r="N57" t="s">
+        <v>35</v>
+      </c>
+      <c r="O57" t="s">
+        <v>420</v>
+      </c>
+      <c r="P57" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>421</v>
+      </c>
+      <c r="R57" t="s">
+        <v>35</v>
+      </c>
+      <c r="S57" t="s">
+        <v>422</v>
+      </c>
+      <c r="T57" t="s">
+        <v>35</v>
+      </c>
+      <c r="U57" t="s">
+        <v>423</v>
+      </c>
+      <c r="W57" t="s">
+        <v>53</v>
+      </c>
+      <c r="X57" t="s">
         <v>65</v>
       </c>
-      <c r="Y58" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="60" spans="12:27">
-      <c r="L60" t="s">
-        <v>316</v>
-      </c>
-      <c r="M60" t="s">
-        <v>317</v>
-      </c>
-      <c r="N60" t="s">
-        <v>35</v>
-      </c>
-      <c r="O60" t="s">
-        <v>318</v>
-      </c>
-      <c r="P60" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>319</v>
-      </c>
-      <c r="R60" t="s">
-        <v>35</v>
-      </c>
-      <c r="S60" t="s">
-        <v>320</v>
-      </c>
-      <c r="T60" t="s">
-        <v>35</v>
-      </c>
-      <c r="W60" t="s">
-        <v>77</v>
-      </c>
-      <c r="X60" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y60" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="62" spans="12:27">
-      <c r="L62" t="s">
-        <v>321</v>
-      </c>
-      <c r="M62" t="s">
-        <v>322</v>
-      </c>
-      <c r="N62" t="s">
-        <v>35</v>
-      </c>
-      <c r="O62" t="s">
-        <v>323</v>
-      </c>
-      <c r="P62" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>324</v>
-      </c>
-      <c r="R62" t="s">
-        <v>35</v>
-      </c>
-      <c r="S62" t="s">
-        <v>325</v>
-      </c>
-      <c r="T62" t="s">
-        <v>35</v>
-      </c>
-      <c r="U62" t="s">
-        <v>326</v>
-      </c>
-      <c r="W62" t="s">
-        <v>77</v>
-      </c>
-      <c r="X62" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y62" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA62" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="64" spans="12:27">
-      <c r="L64" t="s">
-        <v>328</v>
-      </c>
-      <c r="M64" t="s">
-        <v>329</v>
-      </c>
-      <c r="N64" t="s">
-        <v>35</v>
-      </c>
-      <c r="O64" t="s">
-        <v>330</v>
-      </c>
-      <c r="P64" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q64" t="s">
-        <v>331</v>
-      </c>
-      <c r="R64" t="s">
-        <v>35</v>
-      </c>
-      <c r="S64" t="s">
-        <v>332</v>
-      </c>
-      <c r="T64" t="s">
-        <v>35</v>
-      </c>
-      <c r="W64" t="s">
-        <v>53</v>
-      </c>
-      <c r="X64" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y64" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="66" spans="12:25">
-      <c r="L66" t="s">
-        <v>333</v>
-      </c>
-      <c r="M66" t="s">
-        <v>334</v>
-      </c>
-      <c r="N66" t="s">
-        <v>35</v>
-      </c>
-      <c r="O66" t="s">
-        <v>335</v>
-      </c>
-      <c r="P66" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>336</v>
-      </c>
-      <c r="R66" t="s">
-        <v>35</v>
-      </c>
-      <c r="S66" t="s">
-        <v>337</v>
-      </c>
-      <c r="T66" t="s">
-        <v>35</v>
-      </c>
-      <c r="U66" t="s">
-        <v>338</v>
-      </c>
-      <c r="W66" t="s">
-        <v>53</v>
-      </c>
-      <c r="X66" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y66" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="68" spans="12:25">
-      <c r="L68" t="s">
-        <v>339</v>
-      </c>
-      <c r="M68" t="s">
-        <v>340</v>
-      </c>
-      <c r="N68" t="s">
-        <v>35</v>
-      </c>
-      <c r="O68" t="s">
-        <v>341</v>
-      </c>
-      <c r="P68" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q68" t="s">
-        <v>342</v>
-      </c>
-      <c r="R68" t="s">
-        <v>35</v>
-      </c>
-      <c r="S68" t="s">
-        <v>343</v>
-      </c>
-      <c r="T68" t="s">
-        <v>35</v>
-      </c>
-      <c r="W68" t="s">
-        <v>53</v>
-      </c>
-      <c r="X68" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y68" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="70" spans="12:25">
-      <c r="L70" t="s">
-        <v>344</v>
-      </c>
-      <c r="M70" t="s">
-        <v>345</v>
-      </c>
-      <c r="N70" t="s">
-        <v>35</v>
-      </c>
-      <c r="O70" t="s">
-        <v>346</v>
-      </c>
-      <c r="P70" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>347</v>
-      </c>
-      <c r="R70" t="s">
-        <v>35</v>
-      </c>
-      <c r="S70" t="s">
-        <v>348</v>
-      </c>
-      <c r="T70" t="s">
-        <v>35</v>
-      </c>
-      <c r="U70" t="s">
-        <v>349</v>
-      </c>
-      <c r="W70" t="s">
-        <v>53</v>
-      </c>
-      <c r="X70" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y70" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="72" spans="12:25">
-      <c r="L72" t="s">
-        <v>350</v>
-      </c>
-      <c r="M72" t="s">
-        <v>351</v>
-      </c>
-      <c r="N72" t="s">
-        <v>35</v>
-      </c>
-      <c r="O72" t="s">
-        <v>352</v>
-      </c>
-      <c r="P72" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q72" t="s">
-        <v>353</v>
-      </c>
-      <c r="R72" t="s">
-        <v>35</v>
-      </c>
-      <c r="S72" t="s">
-        <v>354</v>
-      </c>
-      <c r="T72" t="s">
-        <v>35</v>
-      </c>
-      <c r="U72" t="s">
-        <v>355</v>
-      </c>
-      <c r="W72" t="s">
-        <v>53</v>
-      </c>
-      <c r="X72" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y72" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="74" spans="12:25">
-      <c r="L74" t="s">
-        <v>356</v>
-      </c>
-      <c r="M74" t="s">
-        <v>357</v>
-      </c>
-      <c r="N74" t="s">
-        <v>35</v>
-      </c>
-      <c r="O74" t="s">
-        <v>358</v>
-      </c>
-      <c r="P74" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q74" t="s">
-        <v>359</v>
-      </c>
-      <c r="R74" t="s">
-        <v>35</v>
-      </c>
-      <c r="S74" t="s">
-        <v>360</v>
-      </c>
-      <c r="T74" t="s">
-        <v>35</v>
-      </c>
-      <c r="U74" t="s">
-        <v>361</v>
-      </c>
-      <c r="W74" t="s">
-        <v>39</v>
-      </c>
-      <c r="X74" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y74" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="76" spans="12:25">
-      <c r="L76" t="s">
-        <v>362</v>
-      </c>
-      <c r="M76" t="s">
-        <v>363</v>
-      </c>
-      <c r="N76" t="s">
-        <v>35</v>
-      </c>
-      <c r="O76" t="s">
-        <v>364</v>
-      </c>
-      <c r="P76" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q76" t="s">
-        <v>365</v>
-      </c>
-      <c r="R76" t="s">
-        <v>35</v>
-      </c>
-      <c r="S76" t="s">
-        <v>366</v>
-      </c>
-      <c r="T76" t="s">
-        <v>35</v>
-      </c>
-      <c r="W76" t="s">
-        <v>53</v>
-      </c>
-      <c r="X76" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y76" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="78" spans="12:25">
-      <c r="L78" t="s">
-        <v>367</v>
-      </c>
-      <c r="M78" t="s">
-        <v>368</v>
-      </c>
-      <c r="N78" t="s">
-        <v>35</v>
-      </c>
-      <c r="O78" t="s">
-        <v>369</v>
-      </c>
-      <c r="P78" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q78" t="s">
-        <v>370</v>
-      </c>
-      <c r="R78" t="s">
-        <v>35</v>
-      </c>
-      <c r="S78" t="s">
-        <v>371</v>
-      </c>
-      <c r="T78" t="s">
-        <v>35</v>
-      </c>
-      <c r="U78" t="s">
-        <v>372</v>
-      </c>
-      <c r="W78" t="s">
-        <v>65</v>
-      </c>
-      <c r="X78" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y78" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="80" spans="12:25">
-      <c r="L80" t="s">
-        <v>373</v>
-      </c>
-      <c r="M80" t="s">
-        <v>374</v>
-      </c>
-      <c r="N80" t="s">
-        <v>35</v>
-      </c>
-      <c r="O80" t="s">
-        <v>375</v>
-      </c>
-      <c r="P80" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q80" t="s">
-        <v>376</v>
-      </c>
-      <c r="R80" t="s">
-        <v>35</v>
-      </c>
-      <c r="S80" t="s">
-        <v>377</v>
-      </c>
-      <c r="T80" t="s">
-        <v>35</v>
-      </c>
-      <c r="W80" t="s">
-        <v>53</v>
-      </c>
-      <c r="X80" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y80" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="82" spans="12:25">
-      <c r="L82" t="s">
-        <v>378</v>
-      </c>
-      <c r="M82" t="s">
-        <v>379</v>
-      </c>
-      <c r="N82" t="s">
-        <v>35</v>
-      </c>
-      <c r="O82" t="s">
-        <v>380</v>
-      </c>
-      <c r="P82" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q82" t="s">
-        <v>381</v>
-      </c>
-      <c r="R82" t="s">
-        <v>35</v>
-      </c>
-      <c r="S82" t="s">
-        <v>382</v>
-      </c>
-      <c r="T82" t="s">
-        <v>35</v>
-      </c>
-      <c r="U82" t="s">
-        <v>383</v>
-      </c>
-      <c r="W82" t="s">
-        <v>65</v>
-      </c>
-      <c r="X82" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y82" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="84" spans="12:25">
-      <c r="L84" t="s">
-        <v>384</v>
-      </c>
-      <c r="M84" t="s">
-        <v>385</v>
-      </c>
-      <c r="N84" t="s">
-        <v>35</v>
-      </c>
-      <c r="O84" t="s">
-        <v>386</v>
-      </c>
-      <c r="P84" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q84" t="s">
-        <v>387</v>
-      </c>
-      <c r="R84" t="s">
-        <v>35</v>
-      </c>
-      <c r="S84" t="s">
-        <v>388</v>
-      </c>
-      <c r="T84" t="s">
-        <v>35</v>
-      </c>
-      <c r="U84" t="s">
-        <v>389</v>
-      </c>
-      <c r="W84" t="s">
-        <v>65</v>
-      </c>
-      <c r="X84" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y84" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="86" spans="12:25">
-      <c r="L86" t="s">
-        <v>390</v>
-      </c>
-      <c r="M86" t="s">
-        <v>391</v>
-      </c>
-      <c r="N86" t="s">
-        <v>35</v>
-      </c>
-      <c r="O86" t="s">
-        <v>392</v>
-      </c>
-      <c r="P86" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q86" t="s">
-        <v>393</v>
-      </c>
-      <c r="R86" t="s">
-        <v>35</v>
-      </c>
-      <c r="S86" t="s">
-        <v>394</v>
-      </c>
-      <c r="T86" t="s">
-        <v>35</v>
-      </c>
-      <c r="U86" t="s">
-        <v>288</v>
-      </c>
-      <c r="W86" t="s">
-        <v>53</v>
-      </c>
-      <c r="X86" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y86" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="88" spans="12:25">
-      <c r="L88" t="s">
-        <v>395</v>
-      </c>
-      <c r="M88" t="s">
-        <v>396</v>
-      </c>
-      <c r="N88" t="s">
-        <v>35</v>
-      </c>
-      <c r="O88" t="s">
-        <v>397</v>
-      </c>
-      <c r="P88" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q88" t="s">
-        <v>398</v>
-      </c>
-      <c r="R88" t="s">
-        <v>35</v>
-      </c>
-      <c r="S88" t="s">
-        <v>399</v>
-      </c>
-      <c r="T88" t="s">
-        <v>35</v>
-      </c>
-      <c r="U88" t="s">
-        <v>400</v>
-      </c>
-      <c r="W88" t="s">
-        <v>53</v>
-      </c>
-      <c r="X88" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y88" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="90" spans="12:25">
-      <c r="L90" t="s">
-        <v>401</v>
-      </c>
-      <c r="M90" t="s">
-        <v>402</v>
-      </c>
-      <c r="N90" t="s">
-        <v>35</v>
-      </c>
-      <c r="O90" t="s">
-        <v>403</v>
-      </c>
-      <c r="P90" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q90" t="s">
-        <v>404</v>
-      </c>
-      <c r="R90" t="s">
-        <v>35</v>
-      </c>
-      <c r="S90" t="s">
-        <v>405</v>
-      </c>
-      <c r="T90" t="s">
-        <v>35</v>
-      </c>
-      <c r="U90" t="s">
-        <v>406</v>
-      </c>
-      <c r="W90" t="s">
-        <v>53</v>
-      </c>
-      <c r="X90" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y90" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="92" spans="12:25">
-      <c r="L92" t="s">
-        <v>407</v>
-      </c>
-      <c r="M92" t="s">
-        <v>408</v>
-      </c>
-      <c r="N92" t="s">
-        <v>35</v>
-      </c>
-      <c r="O92" t="s">
-        <v>409</v>
-      </c>
-      <c r="P92" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q92" t="s">
-        <v>410</v>
-      </c>
-      <c r="R92" t="s">
-        <v>35</v>
-      </c>
-      <c r="S92" t="s">
-        <v>411</v>
-      </c>
-      <c r="T92" t="s">
-        <v>35</v>
-      </c>
-      <c r="U92" t="s">
-        <v>412</v>
-      </c>
-      <c r="W92" t="s">
-        <v>53</v>
-      </c>
-      <c r="X92" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y92" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="94" spans="12:25">
-      <c r="L94" t="s">
-        <v>413</v>
-      </c>
-      <c r="M94" t="s">
-        <v>414</v>
-      </c>
-      <c r="N94" t="s">
-        <v>35</v>
-      </c>
-      <c r="O94" t="s">
-        <v>415</v>
-      </c>
-      <c r="P94" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q94" t="s">
-        <v>416</v>
-      </c>
-      <c r="R94" t="s">
-        <v>35</v>
-      </c>
-      <c r="S94" t="s">
-        <v>417</v>
-      </c>
-      <c r="T94" t="s">
-        <v>35</v>
-      </c>
-      <c r="U94" t="s">
-        <v>418</v>
-      </c>
-      <c r="W94" t="s">
-        <v>53</v>
-      </c>
-      <c r="X94" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y94" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="96" spans="12:25">
-      <c r="L96" t="s">
-        <v>419</v>
-      </c>
-      <c r="M96" t="s">
-        <v>420</v>
-      </c>
-      <c r="N96" t="s">
-        <v>35</v>
-      </c>
-      <c r="O96" t="s">
-        <v>421</v>
-      </c>
-      <c r="P96" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q96" t="s">
-        <v>422</v>
-      </c>
-      <c r="R96" t="s">
-        <v>35</v>
-      </c>
-      <c r="S96" t="s">
-        <v>423</v>
-      </c>
-      <c r="T96" t="s">
-        <v>35</v>
-      </c>
-      <c r="U96" t="s">
-        <v>424</v>
-      </c>
-      <c r="W96" t="s">
-        <v>53</v>
-      </c>
-      <c r="X96" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y96" t="s">
+      <c r="Y57" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>